<commit_message>
Avance en asignación "Carga conciliación manual", scroll del gridview funcionando correctamente
</commit_message>
<xml_diff>
--- a/Conciliacion/App_Web/Sitio Conicliacion 07-07-2017/SitioConciliacion/ControlesUsuario/CargaManualExcelCyC/Excel/Libro1.xlsx
+++ b/Conciliacion/App_Web/Sitio Conicliacion 07-07-2017/SitioConciliacion/ControlesUsuario/CargaManualExcelCyC/Excel/Libro1.xlsx
@@ -32,7 +32,7 @@
     <t>Monto</t>
   </si>
   <si>
-    <t>Cuentass</t>
+    <t>Cuenta</t>
   </si>
 </sst>
 </file>
@@ -354,7 +354,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -372,13 +372,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>656501</v>
+        <v>555</v>
       </c>
       <c r="B2">
         <v>12301</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>